<commit_message>
Develop test data showing CAM assessments
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="409">
   <si>
     <t>Path</t>
   </si>
@@ -512,10 +512,7 @@
     <t>Used for filtering what observations are retrieved and displayed.</t>
   </si>
   <si>
-    <t>Codes for high level observation categories.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-category</t>
+    <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode="COMP].target[classCode="LIST", moodCode="EVN"].code</t>
@@ -1482,7 +1479,7 @@
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.40625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="57.1328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
@@ -3159,10 +3156,10 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>45</v>
@@ -3213,11 +3210,9 @@
       <c r="W15" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="X15" t="s" s="2">
+      <c r="X15" s="2"/>
+      <c r="Y15" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>159</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3259,10 +3254,10 @@
         <v>45</v>
       </c>
       <c r="AM15" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AN15" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="AN15" t="s" s="2">
-        <v>161</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3270,11 +3265,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3296,16 +3291,16 @@
         <v>153</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="M16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>167</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3330,11 +3325,11 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" t="s" s="2">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3352,7 +3347,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>55</v>
@@ -3367,27 +3362,27 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>170</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="AL16" t="s" s="2">
+      <c r="AM16" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="AM16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="AN16" t="s" s="2">
+      <c r="AO16" t="s" s="2">
         <v>174</v>
-      </c>
-      <c r="AO16" t="s" s="2">
-        <v>175</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3410,19 +3405,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>178</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>180</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>181</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3471,7 +3466,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3486,19 +3481,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL17" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="AK17" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AM17" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="AM17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>184</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>185</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3506,7 +3501,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3529,16 +3524,16 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>188</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3588,7 +3583,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3609,13 +3604,13 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3623,11 +3618,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3646,19 +3641,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="M19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>198</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3707,7 +3702,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3722,19 +3717,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL19" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="AK19" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL19" t="s" s="2">
+      <c r="AM19" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="AM19" t="s" s="2">
+      <c r="AN19" t="s" s="2">
         <v>201</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>202</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3742,11 +3737,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3765,19 +3760,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>206</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="M20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>209</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3826,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3841,19 +3836,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL20" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="AK20" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL20" t="s" s="2">
+      <c r="AM20" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="AM20" t="s" s="2">
+      <c r="AN20" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3861,7 +3856,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3884,16 +3879,16 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>218</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3943,7 +3938,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3964,13 +3959,13 @@
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="AM21" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -3978,7 +3973,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4001,17 +3996,17 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>225</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4060,7 +4055,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4075,19 +4070,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AK22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL22" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AK22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AM22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>230</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4095,7 +4090,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4121,16 +4116,16 @@
         <v>153</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>235</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4179,7 +4174,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4188,7 +4183,7 @@
         <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
@@ -4197,24 +4192,24 @@
         <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="AL23" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="AL23" t="s" s="2">
+      <c r="AM23" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="AM23" t="s" s="2">
+      <c r="AN23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO23" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>240</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4240,16 +4235,16 @@
         <v>153</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4274,14 +4269,14 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X24" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="Y24" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="Y24" t="s" s="2">
-        <v>247</v>
-      </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4307,7 +4302,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4322,7 +4317,7 @@
         <v>98</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
@@ -4333,11 +4328,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4359,16 +4354,16 @@
         <v>153</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="M25" t="s" s="2">
+      <c r="N25" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4393,14 +4388,14 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X25" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="Y25" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="Y25" t="s" s="2">
-        <v>257</v>
-      </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4417,7 +4412,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4435,24 +4430,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AL25" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AL25" t="s" s="2">
+      <c r="AM25" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="AM25" t="s" s="2">
+      <c r="AN25" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO25" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO25" t="s" s="2">
-        <v>261</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4475,19 +4470,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4536,7 +4531,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4557,10 +4552,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AM26" t="s" s="2">
         <v>268</v>
-      </c>
-      <c r="AM26" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4571,7 +4566,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4597,13 +4592,13 @@
         <v>153</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4629,14 +4624,14 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="X27" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="X27" t="s" s="2">
+      <c r="Y27" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>276</v>
-      </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4653,7 +4648,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4671,24 +4666,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="AL27" t="s" s="2">
+      <c r="AM27" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="AM27" t="s" s="2">
+      <c r="AN27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO27" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="AN27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO27" t="s" s="2">
-        <v>280</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4714,16 +4709,16 @@
         <v>153</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="M28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>284</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>285</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4748,14 +4743,14 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X28" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="Y28" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="Y28" t="s" s="2">
-        <v>287</v>
-      </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4772,7 +4767,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4793,10 +4788,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AM28" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4807,7 +4802,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4830,16 +4825,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4889,7 +4884,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4907,24 +4902,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>298</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4947,16 +4942,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5006,7 +5001,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5024,24 +5019,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="AL30" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="AL30" t="s" s="2">
+      <c r="AM30" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO30" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>307</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5064,19 +5059,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5125,7 +5120,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5137,19 +5132,19 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="AJ31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5160,7 +5155,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5186,10 +5181,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5240,7 +5235,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5264,7 +5259,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5275,7 +5270,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5304,7 +5299,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5357,7 +5352,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5381,7 +5376,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5392,11 +5387,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5418,10 +5413,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5476,7 +5471,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5511,7 +5506,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5534,13 +5529,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="L35" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5591,7 +5586,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5600,7 +5595,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5612,10 +5607,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5626,7 +5621,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5649,13 +5644,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5706,7 +5701,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5715,7 +5710,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5727,10 +5722,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5741,7 +5736,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5767,16 +5762,16 @@
         <v>153</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5804,11 +5799,11 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="Y37" t="s" s="2">
         <v>346</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>347</v>
-      </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5825,7 +5820,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5843,13 +5838,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AL37" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="AM37" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5860,7 +5855,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5886,16 +5881,16 @@
         <v>153</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5920,14 +5915,14 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="Y38" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="Y38" t="s" s="2">
-        <v>356</v>
-      </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5944,7 +5939,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5962,13 +5957,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AL38" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="AM38" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5979,7 +5974,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6002,17 +5997,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>360</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6061,7 +6056,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6085,7 +6080,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6096,7 +6091,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6122,10 +6117,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6176,7 +6171,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6197,10 +6192,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6211,7 +6206,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6234,16 +6229,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6293,7 +6288,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6314,10 +6309,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6328,7 +6323,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6351,16 +6346,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>375</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6410,7 +6405,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6431,10 +6426,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6445,7 +6440,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6468,19 +6463,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>383</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>384</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6529,7 +6524,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6550,10 +6545,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AM43" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AM43" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6564,7 +6559,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6590,10 +6585,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6644,7 +6639,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6668,7 +6663,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6679,7 +6674,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6708,7 +6703,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6761,7 +6756,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6785,7 +6780,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6796,11 +6791,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6822,10 +6817,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -6880,7 +6875,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6915,7 +6910,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6941,16 +6936,16 @@
         <v>153</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="M47" t="s" s="2">
-        <v>393</v>
-      </c>
       <c r="N47" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6975,14 +6970,14 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X47" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="Y47" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="Y47" t="s" s="2">
-        <v>395</v>
-      </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
       </c>
@@ -6999,7 +6994,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7017,16 +7012,16 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AL47" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="AM47" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="AM47" t="s" s="2">
+      <c r="AN47" t="s" s="2">
         <v>173</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>174</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7034,7 +7029,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7057,19 +7052,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="L48" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>400</v>
-      </c>
       <c r="N48" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7118,7 +7113,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7136,24 +7131,24 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AL48" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="AM48" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="AM48" t="s" s="2">
+      <c r="AN48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>240</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7179,16 +7174,16 @@
         <v>153</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="M49" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="N49" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7213,14 +7208,14 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X49" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="Y49" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="Y49" t="s" s="2">
-        <v>247</v>
-      </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7237,7 +7232,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7246,7 +7241,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7261,7 +7256,7 @@
         <v>98</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7272,11 +7267,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7298,16 +7293,16 @@
         <v>153</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="M50" t="s" s="2">
+      <c r="N50" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7332,14 +7327,14 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X50" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="Y50" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="Y50" t="s" s="2">
-        <v>257</v>
-      </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
       </c>
@@ -7356,7 +7351,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7374,24 +7369,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AL50" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AL50" t="s" s="2">
+      <c r="AM50" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="AM50" t="s" s="2">
+      <c r="AN50" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>261</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7417,16 +7412,16 @@
         <v>45</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="L51" t="s" s="2">
-        <v>409</v>
-      </c>
       <c r="M51" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="N51" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7475,7 +7470,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7496,10 +7491,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Add instances for Connectathon
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$52</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="423">
   <si>
     <t>Path</t>
   </si>
@@ -328,33 +328,66 @@
     <t>Observation.extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>event-location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {event-location}
+</t>
+  </si>
+  <si>
+    <t>Where event occurred</t>
+  </si>
+  <si>
+    <t>The principal physical location where the {{title}} was performed.</t>
+  </si>
+  <si>
+    <t>May reference only *Provenance* resources deemed “relevant” or important. This element does not point to the Provenance associated with the current version of the resource - as it would be created after this version existed. The Provenance for the current version can be retrieved with a [` _revinclude`](search.html#revinclude).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>Event.location</t>
+  </si>
+  <si>
+    <t>EVN.7</t>
+  </si>
+  <si>
+    <t>.participation[typeCode=LOC].role</t>
+  </si>
+  <si>
+    <t>Observation.modifierExtension</t>
+  </si>
+  <si>
     <t>extensions
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Observation.modifierExtension</t>
-  </si>
-  <si>
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
@@ -362,6 +395,9 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
     <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
@@ -512,6 +548,9 @@
     <t>Used for filtering what observations are retrieved and displayed.</t>
   </si>
   <si>
+    <t>If this is from a Post-Acute Care Assessment, value should be survey.</t>
+  </si>
+  <si>
     <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
   </si>
   <si>
@@ -656,8 +695,8 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">dateTime
-</t>
+    <t>dateTime
+PeriodTiminginstant</t>
   </si>
   <si>
     <t>Clinically relevant time/time-period for observation</t>
@@ -740,6 +779,10 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
+    <t>Quantity
+CodeableConcept</t>
+  </si>
+  <si>
     <t>Actual result</t>
   </si>
   <si>
@@ -1021,6 +1064,9 @@
   </si>
   <si>
     <t>Observation.referenceRange.extension</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
   </si>
   <si>
     <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
@@ -1446,7 +1492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO51"/>
+  <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1456,7 +1502,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="44.67578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.19921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
@@ -1478,7 +1524,7 @@
     <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="64.703125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="57.1328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
@@ -2446,7 +2492,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -2465,17 +2511,15 @@
         <v>45</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="L9" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>104</v>
-      </c>
+      <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
         <v>45</v>
@@ -2512,16 +2556,14 @@
         <v>45</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB9" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="AE9" t="s" s="2">
         <v>105</v>
@@ -2548,7 +2590,7 @@
         <v>45</v>
       </c>
       <c r="AM9" t="s" s="2">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="AN9" t="s" s="2">
         <v>45</v>
@@ -2557,45 +2599,45 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>45</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>45</v>
       </c>
@@ -2643,7 +2685,7 @@
         <v>45</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>43</v>
@@ -2652,22 +2694,22 @@
         <v>44</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="AI10" t="s" s="2">
         <v>106</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="AN10" t="s" s="2">
         <v>45</v>
@@ -2678,11 +2720,11 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2695,23 +2737,25 @@
         <v>45</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M11" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="M11" t="s" s="2">
+        <v>120</v>
+      </c>
       <c r="N11" t="s" s="2">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>45</v>
@@ -2760,7 +2804,7 @@
         <v>45</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>43</v>
@@ -2772,22 +2816,22 @@
         <v>45</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="AO11" t="s" s="2">
         <v>45</v>
@@ -2795,11 +2839,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2818,17 +2862,17 @@
         <v>56</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>45</v>
@@ -2877,7 +2921,7 @@
         <v>45</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>43</v>
@@ -2892,19 +2936,19 @@
         <v>67</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="AO12" t="s" s="2">
         <v>45</v>
@@ -2912,11 +2956,11 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
@@ -2935,18 +2979,18 @@
         <v>56</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="N13" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" t="s" s="2">
+        <v>137</v>
+      </c>
       <c r="O13" t="s" s="2">
         <v>45</v>
       </c>
@@ -2994,7 +3038,7 @@
         <v>45</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>43</v>
@@ -3009,16 +3053,16 @@
         <v>67</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>45</v>
@@ -3029,43 +3073,41 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I14" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>143</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
         <v>45</v>
       </c>
@@ -3089,13 +3131,13 @@
         <v>45</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>45</v>
@@ -3113,13 +3155,13 @@
         <v>45</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH14" t="s" s="2">
         <v>45</v>
@@ -3131,16 +3173,16 @@
         <v>147</v>
       </c>
       <c r="AK14" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL14" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="AL14" t="s" s="2">
+      <c r="AM14" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="AM14" t="s" s="2">
-        <v>150</v>
-      </c>
       <c r="AN14" t="s" s="2">
-        <v>151</v>
+        <v>45</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>45</v>
@@ -3148,7 +3190,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3165,25 +3207,25 @@
         <v>45</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K15" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="L15" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="M15" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="N15" t="s" s="2">
         <v>154</v>
-      </c>
-      <c r="L15" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>157</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>45</v>
@@ -3208,11 +3250,13 @@
         <v>45</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="X15" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="X15" t="s" s="2">
+        <v>156</v>
+      </c>
       <c r="Y15" t="s" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3230,13 +3274,13 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>45</v>
@@ -3245,19 +3289,19 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3265,11 +3309,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>162</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3285,22 +3329,22 @@
         <v>45</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3325,11 +3369,13 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="X16" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="X16" t="s" s="2">
+        <v>169</v>
+      </c>
       <c r="Y16" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3347,13 +3393,13 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>45</v>
@@ -3362,31 +3408,31 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="AL16" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="AM16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="AN16" t="s" s="2">
-        <v>173</v>
-      </c>
       <c r="AO16" t="s" s="2">
-        <v>174</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>45</v>
+        <v>174</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3405,19 +3451,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>178</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>180</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3442,13 +3488,11 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X17" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="X17" s="2"/>
       <c r="Y17" t="s" s="2">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3466,10 +3510,10 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>55</v>
@@ -3484,24 +3528,24 @@
         <v>181</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>45</v>
+        <v>182</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>45</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3509,10 +3553,10 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>45</v>
@@ -3524,18 +3568,20 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="N18" s="2"/>
+        <v>191</v>
+      </c>
+      <c r="N18" t="s" s="2">
+        <v>192</v>
+      </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
       </c>
@@ -3583,13 +3629,13 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>45</v>
@@ -3598,19 +3644,19 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>45</v>
+        <v>193</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3618,18 +3664,18 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>45</v>
@@ -3641,20 +3687,18 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>197</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>45</v>
       </c>
@@ -3702,13 +3746,13 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>45</v>
@@ -3717,19 +3761,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>198</v>
+        <v>45</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3737,11 +3781,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3760,19 +3804,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3821,7 +3865,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3836,19 +3880,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3856,11 +3900,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>45</v>
+        <v>215</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3879,18 +3923,20 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N21" s="2"/>
+        <v>219</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
       </c>
@@ -3938,7 +3984,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3953,19 +3999,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -3973,7 +4019,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3981,10 +4027,10 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s" s="2">
         <v>55</v>
-      </c>
-      <c r="F22" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>45</v>
@@ -3996,18 +4042,18 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" t="s" s="2">
-        <v>225</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>45</v>
       </c>
@@ -4055,13 +4101,13 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>45</v>
@@ -4070,19 +4116,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>226</v>
+        <v>45</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4090,7 +4136,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4098,10 +4144,10 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4113,19 +4159,17 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>153</v>
+        <v>234</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>233</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4174,42 +4218,42 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>235</v>
+        <v>45</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>236</v>
+        <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>45</v>
+        <v>241</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>239</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4229,22 +4273,22 @@
         <v>45</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4269,13 +4313,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>167</v>
+        <v>45</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>245</v>
+        <v>45</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>246</v>
+        <v>45</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4293,7 +4337,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4302,7 +4346,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4311,35 +4355,35 @@
         <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>45</v>
+        <v>249</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>98</v>
+        <v>250</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>45</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>45</v>
@@ -4351,19 +4395,19 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4388,13 +4432,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4412,16 +4456,16 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4430,28 +4474,28 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>257</v>
+        <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>258</v>
+        <v>98</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>260</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>45</v>
+        <v>263</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4470,19 +4514,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>262</v>
+        <v>164</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4507,13 +4551,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>45</v>
+        <v>268</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>45</v>
+        <v>269</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4531,7 +4575,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4549,24 +4593,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>45</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4577,7 +4621,7 @@
         <v>43</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>45</v>
@@ -4589,18 +4633,20 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>153</v>
+        <v>275</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N27" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>279</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4624,37 +4670,37 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>273</v>
+        <v>45</v>
       </c>
       <c r="X27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE27" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>269</v>
-      </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>45</v>
@@ -4666,24 +4712,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>276</v>
+        <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>279</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4706,20 +4752,18 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>284</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4743,13 +4787,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4767,7 +4811,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4785,24 +4829,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>45</v>
+        <v>289</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>45</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4825,18 +4869,20 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>290</v>
+        <v>164</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>296</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>297</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4860,13 +4906,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>45</v>
+        <v>298</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>45</v>
+        <v>299</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4884,7 +4930,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4902,24 +4948,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>294</v>
+        <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>297</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4942,16 +4988,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5001,7 +5047,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5019,24 +5065,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5047,7 +5093,7 @@
         <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>45</v>
@@ -5059,20 +5105,18 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>312</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>45</v>
       </c>
@@ -5120,42 +5164,42 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>313</v>
+        <v>67</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>45</v>
+        <v>316</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>45</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5166,7 +5210,7 @@
         <v>43</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>45</v>
@@ -5178,16 +5222,20 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>57</v>
+        <v>321</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+        <v>323</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
@@ -5235,19 +5283,19 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>45</v>
@@ -5256,10 +5304,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>45</v>
+        <v>327</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5270,18 +5318,18 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
@@ -5293,17 +5341,15 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>102</v>
+        <v>330</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>104</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5352,19 +5398,19 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>45</v>
@@ -5376,7 +5422,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5387,11 +5433,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>325</v>
+        <v>117</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5404,26 +5450,24 @@
         <v>45</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>45</v>
       </c>
@@ -5471,7 +5515,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5495,7 +5539,7 @@
         <v>45</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>98</v>
+        <v>333</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5506,39 +5550,43 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>45</v>
+        <v>339</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>330</v>
+        <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+        <v>341</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>121</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5586,19 +5634,19 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>333</v>
+        <v>45</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>45</v>
@@ -5607,10 +5655,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>334</v>
+        <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>335</v>
+        <v>98</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5621,7 +5669,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5644,13 +5692,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5701,7 +5749,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5710,7 +5758,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5722,10 +5770,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5736,7 +5784,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5759,20 +5807,16 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>153</v>
+        <v>344</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>344</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5796,13 +5840,13 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>345</v>
+        <v>45</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5820,7 +5864,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5829,7 +5873,7 @@
         <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>45</v>
+        <v>347</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>67</v>
@@ -5838,13 +5882,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>348</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>259</v>
+        <v>353</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5855,7 +5899,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5866,7 +5910,7 @@
         <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>45</v>
@@ -5878,19 +5922,19 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5915,37 +5959,37 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>273</v>
+        <v>79</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="Y38" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="Z38" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA38" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB38" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC38" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD38" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE38" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="Y38" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="Z38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE38" t="s" s="2">
-        <v>349</v>
-      </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>45</v>
@@ -5957,13 +6001,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5974,7 +6018,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5985,7 +6029,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -5997,17 +6041,19 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>357</v>
+        <v>164</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="M39" s="2"/>
+        <v>365</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>366</v>
+      </c>
       <c r="N39" t="s" s="2">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6032,13 +6078,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>45</v>
+        <v>368</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>45</v>
+        <v>369</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6056,13 +6102,13 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
@@ -6074,13 +6120,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>361</v>
+        <v>272</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6091,7 +6137,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6114,16 +6160,18 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>57</v>
+        <v>371</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="N40" t="s" s="2">
+        <v>374</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6171,7 +6219,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6192,10 +6240,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>334</v>
+        <v>45</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6206,7 +6254,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6217,7 +6265,7 @@
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6226,20 +6274,18 @@
         <v>45</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>367</v>
+        <v>57</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>370</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6288,13 +6334,13 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>45</v>
@@ -6309,10 +6355,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6323,7 +6369,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6346,16 +6392,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6405,7 +6451,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6426,10 +6472,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6440,7 +6486,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6463,20 +6509,18 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>308</v>
+        <v>388</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>383</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6524,7 +6568,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6545,10 +6589,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6559,7 +6603,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6570,7 +6614,7 @@
         <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>45</v>
@@ -6579,19 +6623,23 @@
         <v>45</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>57</v>
+        <v>321</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>317</v>
+        <v>394</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>395</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>397</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6639,19 +6687,19 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>319</v>
+        <v>393</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>45</v>
@@ -6660,10 +6708,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>45</v>
+        <v>398</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>320</v>
+        <v>399</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6674,18 +6722,18 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6697,17 +6745,15 @@
         <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>102</v>
+        <v>330</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>104</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -6756,19 +6802,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6780,7 +6826,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6791,11 +6837,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>325</v>
+        <v>117</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6808,26 +6854,24 @@
         <v>45</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -6875,7 +6919,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6899,7 +6943,7 @@
         <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>98</v>
+        <v>333</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6910,42 +6954,42 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>45</v>
+        <v>339</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>391</v>
+        <v>341</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>392</v>
+        <v>120</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6970,13 +7014,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>273</v>
+        <v>45</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>393</v>
+        <v>45</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>394</v>
+        <v>45</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -6994,34 +7038,34 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>389</v>
+        <v>342</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>395</v>
+        <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>173</v>
+        <v>45</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7029,7 +7073,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7037,7 +7081,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F48" t="s" s="2">
         <v>55</v>
@@ -7052,19 +7096,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>397</v>
+        <v>164</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>232</v>
+        <v>405</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>234</v>
+        <v>178</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7089,13 +7133,13 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>45</v>
+        <v>407</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>45</v>
+        <v>408</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7113,10 +7157,10 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>55</v>
@@ -7131,24 +7175,24 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>237</v>
+        <v>183</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>238</v>
+        <v>184</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>45</v>
+        <v>185</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>239</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7168,22 +7212,22 @@
         <v>45</v>
       </c>
       <c r="I49" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>153</v>
+        <v>411</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>403</v>
+        <v>245</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7208,13 +7252,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>167</v>
+        <v>45</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>245</v>
+        <v>45</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>246</v>
+        <v>45</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7232,7 +7276,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7241,7 +7285,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7250,35 +7294,35 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>45</v>
+        <v>414</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>98</v>
+        <v>250</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>45</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>45</v>
@@ -7290,19 +7334,19 @@
         <v>45</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>251</v>
+        <v>416</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>252</v>
+        <v>417</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>253</v>
+        <v>418</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7327,13 +7371,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7351,16 +7395,16 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>45</v>
+        <v>260</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>67</v>
@@ -7369,28 +7413,28 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>257</v>
+        <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>258</v>
+        <v>98</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>260</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>45</v>
+        <v>263</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -7409,19 +7453,19 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>407</v>
+        <v>264</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>408</v>
+        <v>265</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>311</v>
+        <v>266</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>312</v>
+        <v>267</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7446,13 +7490,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>45</v>
+        <v>268</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>45</v>
+        <v>269</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7470,7 +7514,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7488,23 +7532,142 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>314</v>
+        <v>271</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>315</v>
+        <v>272</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="O52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO52" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO51">
+  <autoFilter ref="A1:AO52">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7514,7 +7677,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI50">
+  <conditionalFormatting sqref="A2:AI51">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add PriorLevelOfCognitiveFunction profile and support for two-column display
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="427">
   <si>
     <t>Path</t>
   </si>
@@ -379,6 +379,19 @@
   </si>
   <si>
     <t>.participation[typeCode=LOC].role</t>
+  </si>
+  <si>
+    <t>device-use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://pacioproject.org/StructureDefinition/device-patient-used}
+</t>
+  </si>
+  <si>
+    <t>Optional Extensions Element</t>
+  </si>
+  <si>
+    <t>Optional Extension Element - found in all resources.</t>
   </si>
   <si>
     <t>Observation.modifierExtension</t>
@@ -1492,7 +1505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO52"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2718,13 +2731,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2734,16 +2749,16 @@
         <v>44</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>45</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="K11" t="s" s="2">
         <v>118</v>
@@ -2751,12 +2766,8 @@
       <c r="L11" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="M11" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="N11" t="s" s="2">
-        <v>121</v>
-      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>45</v>
       </c>
@@ -2804,7 +2815,7 @@
         <v>45</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>43</v>
@@ -2813,7 +2824,7 @@
         <v>44</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>106</v>
@@ -2839,11 +2850,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2856,23 +2867,25 @@
         <v>45</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J12" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="L12" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="M12" t="s" s="2">
         <v>124</v>
       </c>
-      <c r="K12" t="s" s="2">
+      <c r="N12" t="s" s="2">
         <v>125</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" t="s" s="2">
-        <v>127</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>45</v>
@@ -2921,7 +2934,7 @@
         <v>45</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>43</v>
@@ -2933,22 +2946,22 @@
         <v>45</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>129</v>
+        <v>45</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="AO12" t="s" s="2">
         <v>45</v>
@@ -2956,11 +2969,11 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
@@ -2979,17 +2992,17 @@
         <v>56</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" t="s" s="2">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>45</v>
@@ -3038,7 +3051,7 @@
         <v>45</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>43</v>
@@ -3053,19 +3066,19 @@
         <v>67</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>45</v>
@@ -3073,11 +3086,11 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -3096,18 +3109,18 @@
         <v>56</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N14" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="O14" t="s" s="2">
         <v>45</v>
       </c>
@@ -3155,7 +3168,7 @@
         <v>45</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>43</v>
@@ -3170,16 +3183,16 @@
         <v>67</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>45</v>
@@ -3190,43 +3203,41 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>154</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>45</v>
       </c>
@@ -3250,13 +3261,13 @@
         <v>45</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>157</v>
+        <v>45</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3274,13 +3285,13 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>45</v>
@@ -3289,19 +3300,19 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>162</v>
+        <v>45</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3309,7 +3320,7 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3326,25 +3337,25 @@
         <v>45</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3369,13 +3380,13 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3393,13 +3404,13 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>45</v>
@@ -3408,19 +3419,19 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3428,11 +3439,11 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>174</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3448,22 +3459,22 @@
         <v>45</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3488,11 +3499,13 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="X17" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>173</v>
+      </c>
       <c r="Y17" t="s" s="2">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3510,13 +3523,13 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>45</v>
@@ -3525,31 +3538,31 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>186</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3568,19 +3581,19 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3605,13 +3618,11 @@
         <v>45</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X18" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>45</v>
@@ -3629,10 +3640,10 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>55</v>
@@ -3644,27 +3655,27 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>45</v>
+        <v>186</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>45</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3672,10 +3683,10 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>45</v>
@@ -3687,18 +3698,20 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="N19" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>196</v>
+      </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
       </c>
@@ -3746,13 +3759,13 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>45</v>
@@ -3761,19 +3774,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>45</v>
+        <v>197</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3781,18 +3794,18 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>204</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>45</v>
@@ -3804,20 +3817,18 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="M20" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="K20" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>209</v>
-      </c>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>45</v>
       </c>
@@ -3865,13 +3876,13 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>45</v>
@@ -3880,19 +3891,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>210</v>
+        <v>45</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3900,11 +3911,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3923,19 +3934,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3984,7 +3995,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3999,19 +4010,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4019,11 +4030,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4042,18 +4053,20 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="N22" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>224</v>
+      </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
       </c>
@@ -4101,7 +4114,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4116,19 +4129,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4136,7 +4149,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4144,10 +4157,10 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s" s="2">
         <v>55</v>
-      </c>
-      <c r="F23" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4159,18 +4172,18 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" t="s" s="2">
-        <v>237</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>45</v>
       </c>
@@ -4218,13 +4231,13 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>45</v>
@@ -4233,19 +4246,19 @@
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>238</v>
+        <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4253,7 +4266,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4261,10 +4274,10 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>45</v>
@@ -4276,19 +4289,17 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>246</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4337,42 +4348,42 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>249</v>
+        <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>45</v>
+        <v>245</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>252</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4392,22 +4403,22 @@
         <v>45</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>164</v>
+        <v>247</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4432,13 +4443,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>259</v>
+        <v>45</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4456,7 +4467,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4465,7 +4476,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4474,35 +4485,35 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>45</v>
+        <v>253</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>98</v>
+        <v>254</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>45</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>45</v>
@@ -4514,19 +4525,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4551,13 +4562,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4575,16 +4586,16 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>67</v>
@@ -4593,28 +4604,28 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>271</v>
+        <v>98</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>273</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -4633,19 +4644,19 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>275</v>
+        <v>168</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4670,13 +4681,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>45</v>
+        <v>272</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4694,7 +4705,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4712,24 +4723,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>45</v>
+        <v>274</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>45</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4740,7 +4751,7 @@
         <v>43</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>45</v>
@@ -4752,18 +4763,20 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>164</v>
+        <v>279</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="N28" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="L28" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4787,13 +4800,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>286</v>
+        <v>45</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>287</v>
+        <v>45</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>288</v>
+        <v>45</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4811,13 +4824,13 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>45</v>
@@ -4829,24 +4842,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>289</v>
+        <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>292</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4869,20 +4882,18 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>297</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4906,31 +4917,31 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE29" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="X29" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="Y29" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="Z29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4948,24 +4959,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>45</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4988,18 +4999,20 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>303</v>
+        <v>168</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="N30" s="2"/>
+        <v>300</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>301</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
@@ -5023,13 +5036,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>45</v>
+        <v>303</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -5047,7 +5060,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5065,24 +5078,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>307</v>
+        <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>310</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5105,16 +5118,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5164,7 +5177,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5182,24 +5195,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5210,7 +5223,7 @@
         <v>43</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>45</v>
@@ -5222,20 +5235,18 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>325</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
@@ -5283,42 +5294,42 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK32" t="s" s="2">
         <v>320</v>
       </c>
-      <c r="AF32" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AL32" t="s" s="2">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>45</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5329,7 +5340,7 @@
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
@@ -5341,16 +5352,20 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+        <v>327</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="N33" t="s" s="2">
+        <v>329</v>
+      </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
       </c>
@@ -5398,31 +5413,31 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AF33" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG33" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI33" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL33" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="AM33" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AF33" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM33" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5433,18 +5448,18 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>45</v>
@@ -5456,17 +5471,15 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="L34" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>120</v>
-      </c>
+      <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5515,31 +5528,31 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AF34" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG34" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL34" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM34" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL34" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5554,7 +5567,7 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>339</v>
+        <v>121</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5567,26 +5580,24 @@
         <v>45</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
         <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="L35" t="s" s="2">
-        <v>341</v>
-      </c>
       <c r="M35" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>121</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5634,7 +5645,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5658,7 +5669,7 @@
         <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>98</v>
+        <v>337</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5669,39 +5680,43 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>45</v>
+        <v>343</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J36" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K36" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="K36" t="s" s="2">
+      <c r="L36" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="L36" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="M36" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>125</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
       </c>
@@ -5749,19 +5764,19 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>45</v>
@@ -5770,10 +5785,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>348</v>
+        <v>45</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>349</v>
+        <v>98</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5784,7 +5799,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5807,13 +5822,13 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5864,7 +5879,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5873,7 +5888,7 @@
         <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>67</v>
@@ -5885,7 +5900,7 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>353</v>
@@ -5922,7 +5937,7 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>164</v>
+        <v>348</v>
       </c>
       <c r="K38" t="s" s="2">
         <v>355</v>
@@ -5930,12 +5945,8 @@
       <c r="L38" t="s" s="2">
         <v>356</v>
       </c>
-      <c r="M38" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>358</v>
-      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -5959,13 +5970,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>360</v>
+        <v>45</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -5992,7 +6003,7 @@
         <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>45</v>
+        <v>351</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>67</v>
@@ -6001,13 +6012,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>361</v>
+        <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>272</v>
+        <v>357</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6018,7 +6029,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6029,7 +6040,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -6041,19 +6052,19 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6078,13 +6089,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>286</v>
+        <v>79</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6102,13 +6113,13 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
@@ -6120,13 +6131,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6137,7 +6148,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6148,7 +6159,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6160,17 +6171,19 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="N40" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" t="s" s="2">
-        <v>374</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6195,13 +6208,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>45</v>
+        <v>372</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>45</v>
+        <v>373</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6219,13 +6232,13 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
@@ -6237,13 +6250,13 @@
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>45</v>
+        <v>366</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>375</v>
+        <v>276</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6254,7 +6267,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6277,16 +6290,18 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>57</v>
+        <v>375</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" s="2"/>
+      <c r="N41" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6334,7 +6349,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6355,7 +6370,7 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>348</v>
+        <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>379</v>
@@ -6380,7 +6395,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>45</v>
@@ -6389,20 +6404,18 @@
         <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>382</v>
       </c>
-      <c r="L42" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>384</v>
-      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>45</v>
@@ -6457,7 +6470,7 @@
         <v>43</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>45</v>
@@ -6472,10 +6485,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>385</v>
+        <v>352</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6486,7 +6499,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6509,16 +6522,16 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>388</v>
-      </c>
-      <c r="K43" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6568,7 +6581,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6589,10 +6602,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6603,7 +6616,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6626,20 +6639,18 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>321</v>
+        <v>392</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M44" t="s" s="2">
-        <v>396</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>397</v>
-      </c>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6687,7 +6698,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6708,10 +6719,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6722,7 +6733,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6733,7 +6744,7 @@
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6742,19 +6753,23 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>57</v>
+        <v>325</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>330</v>
+        <v>398</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>399</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>401</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6802,19 +6817,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>332</v>
+        <v>397</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6823,10 +6838,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>45</v>
+        <v>402</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>333</v>
+        <v>403</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6837,18 +6852,18 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6860,17 +6875,15 @@
         <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="L46" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>120</v>
-      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
@@ -6919,31 +6932,31 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM46" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="AF46" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI46" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AJ46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6954,11 +6967,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>339</v>
+        <v>121</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6971,26 +6984,24 @@
         <v>45</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
         <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="L47" t="s" s="2">
-        <v>341</v>
-      </c>
       <c r="M47" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>121</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
       </c>
@@ -7038,7 +7049,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7062,7 +7073,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>98</v>
+        <v>337</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7073,42 +7084,42 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>45</v>
+        <v>343</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>404</v>
+        <v>344</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>405</v>
+        <v>345</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>406</v>
+        <v>124</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7133,13 +7144,13 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>286</v>
+        <v>45</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>407</v>
+        <v>45</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>408</v>
+        <v>45</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7157,34 +7168,34 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>403</v>
+        <v>346</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>409</v>
+        <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>184</v>
+        <v>98</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>185</v>
+        <v>45</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>45</v>
@@ -7192,7 +7203,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7200,7 +7211,7 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F49" t="s" s="2">
         <v>55</v>
@@ -7215,19 +7226,19 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>411</v>
+        <v>168</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>245</v>
+        <v>409</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>247</v>
+        <v>182</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7252,13 +7263,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>45</v>
+        <v>411</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>45</v>
+        <v>412</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7276,10 +7287,10 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>55</v>
@@ -7294,24 +7305,24 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>250</v>
+        <v>187</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>251</v>
+        <v>188</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>252</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7331,22 +7342,22 @@
         <v>45</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>164</v>
+        <v>415</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>416</v>
       </c>
       <c r="L50" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="M50" t="s" s="2">
-        <v>418</v>
-      </c>
       <c r="N50" t="s" s="2">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7371,13 +7382,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>259</v>
+        <v>45</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7395,7 +7406,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7404,7 +7415,7 @@
         <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>260</v>
+        <v>45</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>67</v>
@@ -7413,19 +7424,19 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>45</v>
+        <v>418</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>98</v>
+        <v>254</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>45</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -7434,14 +7445,14 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>45</v>
@@ -7453,19 +7464,19 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>264</v>
+        <v>420</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>265</v>
+        <v>421</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>266</v>
+        <v>422</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7490,13 +7501,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7520,10 +7531,10 @@
         <v>43</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>67</v>
@@ -7532,28 +7543,28 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>271</v>
+        <v>98</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>273</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7572,19 +7583,19 @@
         <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>45</v>
+        <v>168</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>421</v>
+        <v>268</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>422</v>
+        <v>269</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>324</v>
+        <v>270</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>325</v>
+        <v>271</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7609,13 +7620,13 @@
         <v>45</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>45</v>
+        <v>272</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7633,7 +7644,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7651,23 +7662,142 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>45</v>
+        <v>274</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>327</v>
+        <v>275</v>
       </c>
       <c r="AM52" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO52" t="s" s="2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="AN52" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO52" t="s" s="2">
+      <c r="N53" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO53" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO52">
+  <autoFilter ref="A1:AO53">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7677,7 +7807,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI51">
+  <conditionalFormatting sqref="A2:AI52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add new contents to IG web pages
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="415">
   <si>
     <t>Path</t>
   </si>
@@ -456,7 +456,7 @@
 </t>
   </si>
   <si>
-    <t>Fulfills plan, proposal or order</t>
+    <t>Currently not used in BundledCognitiveStatus.</t>
   </si>
   <si>
     <t>A plan, proposal or order that is fulfilled in whole or in part by this event.  For example, a MedicationRequest may require a patient to have laboratory test performed before  it is dispensed.</t>
@@ -485,9 +485,6 @@
 </t>
   </si>
   <si>
-    <t>Part of referenced event</t>
-  </si>
-  <si>
     <t>A larger event of which this particular Observation is a component or step.  For example,  an observation as part of a procedure.</t>
   </si>
   <si>
@@ -506,7 +503,7 @@
     <t>Observation.status</t>
   </si>
   <si>
-    <t>registered | preliminary | final | amended +</t>
+    <t>Should have the value 'final' to indicate the assessment is complete.</t>
   </si>
   <si>
     <t>The status of the result value.</t>
@@ -549,7 +546,7 @@
 </t>
   </si>
   <si>
-    <t>Classification of  type of observation</t>
+    <t>For a Post-Acute Care Assessment, should have the value 'survey'.</t>
   </si>
   <si>
     <t>A code that classifies the general type of observation being made.</t>
@@ -559,9 +556,6 @@
   </si>
   <si>
     <t>Used for filtering what observations are retrieved and displayed.</t>
-  </si>
-  <si>
-    <t>If this is from a Post-Acute Care Assessment, value should be survey.</t>
   </si>
   <si>
     <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
@@ -580,7 +574,7 @@
 </t>
   </si>
   <si>
-    <t>Type of observation (code / type)</t>
+    <t>For a Post-Acute Care Assessment, should include a LOINC code and text for the kind of assessment.</t>
   </si>
   <si>
     <t>Describes what was observed. Sometimes this is called the observation "name".</t>
@@ -590,9 +584,6 @@
   </si>
   <si>
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
-  </si>
-  <si>
-    <t>extensible</t>
   </si>
   <si>
     <t>http://loinc.org</t>
@@ -623,7 +614,7 @@
 </t>
   </si>
   <si>
-    <t>Who and/or what the observation is about</t>
+    <t>Should only reference a Patient resource</t>
   </si>
   <si>
     <t>The patient, or group of patients, location, or device this observation is about and into whose record the observation is placed. If the actual focus of the observation is different from the subject (or a sample of, part, or region of the subject), the `focus` element or the `code` itself specifies the actual focus of the observation.</t>
@@ -654,9 +645,6 @@
 </t>
   </si>
   <si>
-    <t>What the observation is about, when it is not about the subject of record</t>
-  </si>
-  <si>
     <t>The actual focus of an observation when it is not the patient of record representing something or someone associated with the patient such as a spouse, parent, fetus, or donor. For example, fetus observations in a mother's record.  The focus of an observation could also be an existing condition,  an intervention, the subject's diet,  another observation of the subject,  or a body structure such as tumor or implanted device.   An example use case would be using the Observation resource to capture whether the mother is trained to change her child's tracheostomy tube. In this example, the child is the patient of record and the mother is the focus.</t>
   </si>
   <si>
@@ -709,7 +697,7 @@
   </si>
   <si>
     <t>dateTime
-PeriodTiminginstant</t>
+Period</t>
   </si>
   <si>
     <t>Clinically relevant time/time-period for observation</t>
@@ -743,9 +731,6 @@
 </t>
   </si>
   <si>
-    <t>Date/Time this version was made available</t>
-  </si>
-  <si>
     <t>The date and time this version of the observation was made available to providers, typically after the results have been reviewed and verified.</t>
   </si>
   <si>
@@ -768,7 +753,7 @@
 </t>
   </si>
   <si>
-    <t>Who is responsible for the observation</t>
+    <t xml:space="preserve">The person who performed the assessment. May also be used to provide the practitioner role and organization. </t>
   </si>
   <si>
     <t>Who was responsible for asserting the observed value as "true".</t>
@@ -790,10 +775,6 @@
   </si>
   <si>
     <t>Observation.value[x]</t>
-  </si>
-  <si>
-    <t>Quantity
-CodeableConcept</t>
   </si>
   <si>
     <t>Actual result</t>
@@ -827,9 +808,6 @@
     <t>Observation.dataAbsentReason</t>
   </si>
   <si>
-    <t>Why the result is missing</t>
-  </si>
-  <si>
     <t>Provides a reason why the expected value in the element Observation.value[x] is missing.</t>
   </si>
   <si>
@@ -840,6 +818,9 @@
     <t>For many results it is necessary to handle exceptional values in measurements.</t>
   </si>
   <si>
+    <t>extensible</t>
+  </si>
+  <si>
     <t>Codes specifying why the result (`Observation.value[x]`) is missing.</t>
   </si>
   <si>
@@ -860,9 +841,6 @@
 </t>
   </si>
   <si>
-    <t>High, low, normal, etc.</t>
-  </si>
-  <si>
     <t>A categorical assessment of an observation value.  For example, high, low, normal.</t>
   </si>
   <si>
@@ -918,9 +896,6 @@
     <t>Observation.bodySite</t>
   </si>
   <si>
-    <t>Observed body part</t>
-  </si>
-  <si>
     <t>Indicates the site on the subject's body where the observation was made (i.e. the target site).</t>
   </si>
   <si>
@@ -952,9 +927,6 @@
     <t>Observation.method</t>
   </si>
   <si>
-    <t>How it was done</t>
-  </si>
-  <si>
     <t>Indicates the mechanism used to perform the observation.</t>
   </si>
   <si>
@@ -983,9 +955,6 @@
 </t>
   </si>
   <si>
-    <t>Specimen used for this observation</t>
-  </si>
-  <si>
     <t>The specimen that was used when this observation was made.</t>
   </si>
   <si>
@@ -1011,9 +980,6 @@
 </t>
   </si>
   <si>
-    <t>(Measurement) Device</t>
-  </si>
-  <si>
     <t>The device used to generate the observation data.</t>
   </si>
   <si>
@@ -1037,9 +1003,6 @@
   <si>
     <t xml:space="preserve">BackboneElement
 </t>
-  </si>
-  <si>
-    <t>Provides guide for interpretation</t>
   </si>
   <si>
     <t>Guidance on how to interpret the value by comparison to a normal or recommended range.  Multiple reference ranges are interpreted as an "OR".   In other words, to represent two distinct target populations, two `referenceRange` elements would be used.</t>
@@ -1269,9 +1232,6 @@
     <t>Observation.component</t>
   </si>
   <si>
-    <t>Component results</t>
-  </si>
-  <si>
     <t>Some observations have multiple component observations.  These component observations are expressed as separate code value pairs that share the same attributes.  Examples include systolic and diastolic component observations for blood pressure measurement and multiple component observations for genetics observations.</t>
   </si>
   <si>
@@ -1348,6 +1308,9 @@
   </si>
   <si>
     <t>Observation.component.interpretation</t>
+  </si>
+  <si>
+    <t>High, low, normal, etc.</t>
   </si>
   <si>
     <t>Observation.component.referenceRange</t>
@@ -1524,7 +1487,7 @@
     <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="67.91015625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="104.1484375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1537,7 +1500,7 @@
     <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="64.703125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="57.1328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
@@ -3229,13 +3192,13 @@
         <v>147</v>
       </c>
       <c r="K15" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="L15" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>149</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>150</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3300,16 +3263,16 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AK15" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL15" t="s" s="2">
         <v>151</v>
       </c>
-      <c r="AK15" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL15" t="s" s="2">
+      <c r="AM15" t="s" s="2">
         <v>152</v>
-      </c>
-      <c r="AM15" t="s" s="2">
-        <v>153</v>
       </c>
       <c r="AN15" t="s" s="2">
         <v>45</v>
@@ -3320,7 +3283,7 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3346,16 +3309,16 @@
         <v>75</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="M16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3380,14 +3343,14 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="X16" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="X16" t="s" s="2">
+      <c r="Y16" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="Y16" t="s" s="2">
-        <v>161</v>
-      </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
       </c>
@@ -3404,7 +3367,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>55</v>
@@ -3419,19 +3382,19 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AL16" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="AL16" t="s" s="2">
+      <c r="AM16" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="AM16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>165</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>166</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3439,7 +3402,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3462,19 +3425,19 @@
         <v>45</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>170</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>171</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>172</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3501,11 +3464,9 @@
       <c r="W17" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="X17" t="s" s="2">
-        <v>173</v>
-      </c>
+      <c r="X17" s="2"/>
       <c r="Y17" t="s" s="2">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3523,7 +3484,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3547,10 +3508,10 @@
         <v>45</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3558,11 +3519,11 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3581,19 +3542,19 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K18" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="L18" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="M18" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="N18" t="s" s="2">
         <v>180</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>182</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3618,11 +3579,11 @@
         <v>45</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>183</v>
+        <v>79</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>45</v>
@@ -3640,7 +3601,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>55</v>
@@ -3655,27 +3616,27 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="AL18" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="AM18" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AN18" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="AL18" t="s" s="2">
+      <c r="AO18" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="AN18" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="AO18" t="s" s="2">
-        <v>190</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3698,19 +3659,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="M19" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>196</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3759,7 +3720,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3774,19 +3735,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="AM19" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="AN19" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="AK19" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3794,7 +3755,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3817,16 +3778,16 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>203</v>
+        <v>139</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3876,7 +3837,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3897,13 +3858,13 @@
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3911,11 +3872,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3934,19 +3895,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="N21" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="K21" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3995,7 +3956,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -4010,19 +3971,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4030,11 +3991,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4053,19 +4014,19 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="K22" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="N22" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="K22" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4114,7 +4075,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4129,19 +4090,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4149,7 +4110,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4172,16 +4133,16 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>231</v>
+        <v>139</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4231,7 +4192,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4252,13 +4213,13 @@
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4266,7 +4227,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4289,17 +4250,17 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4348,7 +4309,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4363,19 +4324,19 @@
         <v>67</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4383,7 +4344,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4406,19 +4367,19 @@
         <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>247</v>
+        <v>167</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4467,7 +4428,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4476,7 +4437,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4485,24 +4446,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4525,19 +4486,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>258</v>
+        <v>139</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4562,13 +4523,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4586,7 +4547,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4595,7 +4556,7 @@
         <v>55</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>67</v>
@@ -4610,7 +4571,7 @@
         <v>98</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4621,11 +4582,11 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -4644,19 +4605,19 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>268</v>
+        <v>139</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4681,13 +4642,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4705,7 +4666,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4723,24 +4684,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4763,19 +4724,19 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4824,7 +4785,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4845,10 +4806,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4859,7 +4820,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4882,16 +4843,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>287</v>
+        <v>139</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4917,13 +4878,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4941,7 +4902,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4959,24 +4920,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4999,19 +4960,19 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>298</v>
+        <v>139</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -5036,13 +4997,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -5060,7 +5021,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5081,10 +5042,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5095,7 +5056,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5118,16 +5079,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>308</v>
+        <v>139</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5177,7 +5138,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5195,24 +5156,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5235,16 +5196,16 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>317</v>
+        <v>139</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5294,7 +5255,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5312,24 +5273,24 @@
         <v>45</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5352,19 +5313,19 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>326</v>
+        <v>139</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5413,7 +5374,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5425,7 +5386,7 @@
         <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>45</v>
@@ -5434,10 +5395,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5448,7 +5409,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5474,10 +5435,10 @@
         <v>57</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5528,7 +5489,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5552,7 +5513,7 @@
         <v>45</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5563,7 +5524,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5589,10 +5550,10 @@
         <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="M35" t="s" s="2">
         <v>124</v>
@@ -5645,7 +5606,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5669,7 +5630,7 @@
         <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5680,11 +5641,11 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -5706,10 +5667,10 @@
         <v>100</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="M36" t="s" s="2">
         <v>124</v>
@@ -5764,7 +5725,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5799,7 +5760,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5822,13 +5783,13 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5879,7 +5840,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5888,7 +5849,7 @@
         <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>67</v>
@@ -5900,10 +5861,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5914,7 +5875,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5937,13 +5898,13 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5994,7 +5955,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6003,7 +5964,7 @@
         <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>67</v>
@@ -6015,10 +5976,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6029,7 +5990,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6052,19 +6013,19 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6092,10 +6053,10 @@
         <v>79</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6113,7 +6074,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6131,13 +6092,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6148,7 +6109,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6171,19 +6132,19 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6208,13 +6169,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6232,7 +6193,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6250,13 +6211,13 @@
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6267,7 +6228,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6290,17 +6251,17 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s" s="2">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6349,7 +6310,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6373,7 +6334,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6384,7 +6345,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6410,10 +6371,10 @@
         <v>57</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6464,7 +6425,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6485,10 +6446,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6499,7 +6460,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6522,16 +6483,16 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6581,7 +6542,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6602,10 +6563,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6616,7 +6577,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6639,16 +6600,16 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6698,7 +6659,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6719,10 +6680,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6733,7 +6694,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6756,19 +6717,19 @@
         <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>398</v>
+        <v>139</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -6817,7 +6778,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6838,10 +6799,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6852,7 +6813,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6878,10 +6839,10 @@
         <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6932,7 +6893,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6956,7 +6917,7 @@
         <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6967,7 +6928,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6993,10 +6954,10 @@
         <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>124</v>
@@ -7049,7 +7010,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7073,7 +7034,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7084,11 +7045,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7110,10 +7071,10 @@
         <v>100</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>124</v>
@@ -7168,7 +7129,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7203,7 +7164,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7226,19 +7187,19 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7263,13 +7224,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7287,7 +7248,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>55</v>
@@ -7305,16 +7266,16 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7322,7 +7283,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7345,19 +7306,19 @@
         <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7406,7 +7367,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7424,24 +7385,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7464,19 +7425,19 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7501,13 +7462,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7525,7 +7486,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7534,7 +7495,7 @@
         <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>67</v>
@@ -7549,7 +7510,7 @@
         <v>98</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7560,11 +7521,11 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7583,19 +7544,19 @@
         <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>268</v>
+        <v>411</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7620,13 +7581,13 @@
         <v>45</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7644,7 +7605,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7662,24 +7623,24 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7705,16 +7666,16 @@
         <v>45</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7763,7 +7724,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7784,10 +7745,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Change back to use binding 'extensible' for 'observation.code'
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -558,6 +558,9 @@
     <t>Used for filtering what observations are retrieved and displayed.</t>
   </si>
   <si>
+    <t>extensible</t>
+  </si>
+  <si>
     <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
   </si>
   <si>
@@ -816,9 +819,6 @@
   </si>
   <si>
     <t>For many results it is necessary to handle exceptional values in measurements.</t>
-  </si>
-  <si>
-    <t>extensible</t>
   </si>
   <si>
     <t>Codes specifying why the result (`Observation.value[x]`) is missing.</t>
@@ -3462,11 +3462,11 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>79</v>
+        <v>172</v>
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3508,10 +3508,10 @@
         <v>45</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3519,11 +3519,11 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3545,16 +3545,16 @@
         <v>167</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3579,11 +3579,11 @@
         <v>45</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>79</v>
+        <v>172</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>45</v>
@@ -3601,7 +3601,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>55</v>
@@ -3616,27 +3616,27 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3659,19 +3659,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3720,7 +3720,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3735,19 +3735,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3778,16 +3778,16 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K20" t="s" s="2">
         <v>139</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3837,7 +3837,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3858,13 +3858,13 @@
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3872,11 +3872,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3895,19 +3895,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3956,7 +3956,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3971,19 +3971,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -3991,11 +3991,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4014,19 +4014,19 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4075,7 +4075,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4090,19 +4090,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4133,16 +4133,16 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K23" t="s" s="2">
         <v>139</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4192,7 +4192,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4213,13 +4213,13 @@
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4250,17 +4250,17 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4309,7 +4309,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4324,19 +4324,19 @@
         <v>67</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4344,7 +4344,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4370,16 +4370,16 @@
         <v>167</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4428,7 +4428,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4437,7 +4437,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4446,24 +4446,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4492,13 +4492,13 @@
         <v>139</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4523,7 +4523,7 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>255</v>
+        <v>172</v>
       </c>
       <c r="X26" t="s" s="2">
         <v>256</v>
@@ -4547,7 +4547,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4642,7 +4642,7 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>255</v>
+        <v>172</v>
       </c>
       <c r="X27" t="s" s="2">
         <v>265</v>
@@ -7199,7 +7199,7 @@
         <v>397</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7269,13 +7269,13 @@
         <v>400</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7312,13 +7312,13 @@
         <v>403</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>404</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7388,16 +7388,16 @@
         <v>405</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -7437,7 +7437,7 @@
         <v>409</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7462,7 +7462,7 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>255</v>
+        <v>172</v>
       </c>
       <c r="X51" t="s" s="2">
         <v>256</v>
@@ -7581,7 +7581,7 @@
         <v>45</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>255</v>
+        <v>172</v>
       </c>
       <c r="X52" t="s" s="2">
         <v>265</v>

</xml_diff>

<commit_message>
Use US Core profiles and Fix build errors and warnings
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="424">
   <si>
     <t>Path</t>
   </si>
@@ -546,7 +546,7 @@
 </t>
   </si>
   <si>
-    <t>For a Post-Acute Care Assessment, should have the value 'survey'.</t>
+    <t>Classification of  type of observation</t>
   </si>
   <si>
     <t>A code that classifies the general type of observation being made.</t>
@@ -558,10 +558,10 @@
     <t>Used for filtering what observations are retrieved and displayed.</t>
   </si>
   <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>http://terminology.hl7.org/CodeSystem/observation-category</t>
+    <t>Codes for high level observation categories.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-category</t>
   </si>
   <si>
     <t xml:space="preserve">pattern:$this}
@@ -575,9 +575,6 @@
   </si>
   <si>
     <t>Laboratory</t>
-  </si>
-  <si>
-    <t>Classification of  type of observation</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -588,12 +585,6 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t>Codes for high level observation categories.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-category</t>
-  </si>
-  <si>
     <t>Observation.code</t>
   </si>
   <si>
@@ -611,6 +602,9 @@
   </si>
   <si>
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
+  </si>
+  <si>
+    <t>extensible</t>
   </si>
   <si>
     <t>http://loinc.org</t>
@@ -1544,7 +1538,7 @@
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="63.703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="57.1328125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="50.40625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
@@ -3503,7 +3497,7 @@
         <v>56</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>57</v>
@@ -3552,9 +3546,11 @@
         <v>46</v>
       </c>
       <c r="W17" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X17" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="X17" s="2"/>
       <c r="Y17" t="s" s="2">
         <v>173</v>
       </c>
@@ -3638,7 +3634,7 @@
         <v>167</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="L18" t="s" s="2">
         <v>169</v>
@@ -3657,7 +3653,7 @@
         <v>46</v>
       </c>
       <c r="R18" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S18" t="s" s="2">
         <v>46</v>
@@ -3675,10 +3671,10 @@
         <v>80</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>46</v>
@@ -3734,11 +3730,11 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3760,16 +3756,16 @@
         <v>167</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="N19" t="s" s="2">
         <v>184</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>187</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>46</v>
@@ -3794,11 +3790,11 @@
         <v>46</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="X19" s="2"/>
       <c r="Y19" t="s" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>46</v>
@@ -3816,7 +3812,7 @@
         <v>46</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>56</v>
@@ -3831,30 +3827,30 @@
         <v>68</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AK19" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AM19" t="s" s="2">
         <v>189</v>
       </c>
-      <c r="AL19" t="s" s="2">
+      <c r="AN19" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="AM19" t="s" s="2">
+      <c r="AO19" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="AN19" t="s" s="2">
+      <c r="AP19" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="AO19" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="AP19" t="s" s="2">
-        <v>194</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3877,19 +3873,19 @@
         <v>57</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>198</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>46</v>
@@ -3938,7 +3934,7 @@
         <v>46</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>44</v>
@@ -3953,22 +3949,22 @@
         <v>68</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AK20" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AM20" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AN20" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="AL20" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM20" t="s" s="2">
+      <c r="AO20" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="AO20" t="s" s="2">
-        <v>204</v>
       </c>
       <c r="AP20" t="s" s="2">
         <v>46</v>
@@ -3976,7 +3972,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3999,16 +3995,16 @@
         <v>57</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K21" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -4058,7 +4054,7 @@
         <v>46</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>44</v>
@@ -4082,13 +4078,13 @@
         <v>46</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AP21" t="s" s="2">
         <v>46</v>
@@ -4096,11 +4092,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4119,19 +4115,19 @@
         <v>57</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="K22" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>46</v>
@@ -4180,7 +4176,7 @@
         <v>46</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>44</v>
@@ -4198,19 +4194,19 @@
         <v>46</v>
       </c>
       <c r="AK22" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AM22" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AN22" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="AL22" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM22" t="s" s="2">
+      <c r="AO22" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="AO22" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="AP22" t="s" s="2">
         <v>46</v>
@@ -4218,11 +4214,11 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -4241,19 +4237,19 @@
         <v>57</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>227</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>46</v>
@@ -4302,7 +4298,7 @@
         <v>46</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>44</v>
@@ -4311,28 +4307,28 @@
         <v>56</v>
       </c>
       <c r="AH23" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AI23" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AK23" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AI23" t="s" s="2">
+      <c r="AL23" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AM23" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="AJ23" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="AK23" t="s" s="2">
+      <c r="AN23" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="AL23" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM23" t="s" s="2">
+      <c r="AO23" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="AP23" t="s" s="2">
         <v>46</v>
@@ -4340,7 +4336,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4363,16 +4359,16 @@
         <v>57</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K24" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -4422,7 +4418,7 @@
         <v>46</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>44</v>
@@ -4446,13 +4442,13 @@
         <v>46</v>
       </c>
       <c r="AM24" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="AN24" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="AO24" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="AO24" t="s" s="2">
-        <v>240</v>
       </c>
       <c r="AP24" t="s" s="2">
         <v>46</v>
@@ -4460,7 +4456,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4483,17 +4479,17 @@
         <v>57</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="K25" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="K25" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" t="s" s="2">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>46</v>
@@ -4542,7 +4538,7 @@
         <v>46</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>44</v>
@@ -4560,19 +4556,19 @@
         <v>46</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AM25" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AN25" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="AL25" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM25" t="s" s="2">
+      <c r="AO25" t="s" s="2">
         <v>247</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="AO25" t="s" s="2">
-        <v>249</v>
       </c>
       <c r="AP25" t="s" s="2">
         <v>46</v>
@@ -4580,7 +4576,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4606,16 +4602,16 @@
         <v>167</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="M26" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>46</v>
@@ -4664,7 +4660,7 @@
         <v>46</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>44</v>
@@ -4673,36 +4669,36 @@
         <v>56</v>
       </c>
       <c r="AH26" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="AI26" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AJ26" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AK26" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AL26" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="AI26" t="s" s="2">
+      <c r="AM26" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="AJ26" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="AK26" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL26" t="s" s="2">
+      <c r="AN26" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="AM26" t="s" s="2">
+      <c r="AO26" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AP26" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="AN26" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="AO26" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP26" t="s" s="2">
-        <v>260</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4731,13 +4727,13 @@
         <v>140</v>
       </c>
       <c r="L27" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="N27" t="s" s="2">
         <v>262</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>264</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>46</v>
@@ -4762,11 +4758,11 @@
         <v>46</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="X27" s="2"/>
       <c r="Y27" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>46</v>
@@ -4784,7 +4780,7 @@
         <v>46</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>44</v>
@@ -4793,13 +4789,13 @@
         <v>56</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>68</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>46</v>
@@ -4811,7 +4807,7 @@
         <v>99</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>46</v>
@@ -4822,11 +4818,11 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4851,13 +4847,13 @@
         <v>140</v>
       </c>
       <c r="L28" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="N28" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>46</v>
@@ -4882,13 +4878,13 @@
         <v>46</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>46</v>
@@ -4906,7 +4902,7 @@
         <v>46</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>44</v>
@@ -4927,24 +4923,24 @@
         <v>46</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="AM28" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AN28" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="AM28" t="s" s="2">
+      <c r="AO28" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AP28" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="AN28" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AO28" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP28" t="s" s="2">
-        <v>278</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4967,19 +4963,19 @@
         <v>46</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>46</v>
@@ -5028,7 +5024,7 @@
         <v>46</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>44</v>
@@ -5052,10 +5048,10 @@
         <v>46</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>46</v>
@@ -5066,7 +5062,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5095,10 +5091,10 @@
         <v>140</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5124,14 +5120,14 @@
         <v>46</v>
       </c>
       <c r="W30" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="Y30" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="X30" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="Y30" t="s" s="2">
-        <v>292</v>
-      </c>
       <c r="Z30" t="s" s="2">
         <v>46</v>
       </c>
@@ -5148,7 +5144,7 @@
         <v>46</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>44</v>
@@ -5169,24 +5165,24 @@
         <v>46</v>
       </c>
       <c r="AL30" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AM30" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="AN30" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AO30" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AP30" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP30" t="s" s="2">
-        <v>296</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5215,13 +5211,13 @@
         <v>140</v>
       </c>
       <c r="L31" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="N31" t="s" s="2">
         <v>298</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>46</v>
@@ -5246,13 +5242,13 @@
         <v>46</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>46</v>
@@ -5270,7 +5266,7 @@
         <v>46</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>44</v>
@@ -5294,10 +5290,10 @@
         <v>46</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>46</v>
@@ -5308,7 +5304,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5331,16 +5327,16 @@
         <v>46</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5390,7 +5386,7 @@
         <v>46</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>44</v>
@@ -5411,24 +5407,24 @@
         <v>46</v>
       </c>
       <c r="AL32" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AM32" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AN32" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="AM32" t="s" s="2">
+      <c r="AO32" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AP32" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AN32" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="AO32" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP32" t="s" s="2">
-        <v>312</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5451,16 +5447,16 @@
         <v>46</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K33" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
@@ -5510,7 +5506,7 @@
         <v>46</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>44</v>
@@ -5531,24 +5527,24 @@
         <v>46</v>
       </c>
       <c r="AL33" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AM33" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AN33" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="AM33" t="s" s="2">
+      <c r="AO33" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AP33" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="AN33" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="AO33" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP33" t="s" s="2">
-        <v>320</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5571,19 +5567,19 @@
         <v>46</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K34" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L34" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="N34" t="s" s="2">
         <v>323</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>46</v>
@@ -5632,7 +5628,7 @@
         <v>46</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>44</v>
@@ -5644,22 +5640,22 @@
         <v>46</v>
       </c>
       <c r="AI34" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AK34" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AL34" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AM34" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="AN34" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL34" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="AN34" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>46</v>
@@ -5670,7 +5666,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5696,10 +5692,10 @@
         <v>58</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5750,7 +5746,7 @@
         <v>46</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>44</v>
@@ -5777,7 +5773,7 @@
         <v>46</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>46</v>
@@ -5788,7 +5784,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5814,10 +5810,10 @@
         <v>101</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M36" t="s" s="2">
         <v>125</v>
@@ -5870,7 +5866,7 @@
         <v>46</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>44</v>
@@ -5897,7 +5893,7 @@
         <v>46</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>46</v>
@@ -5908,11 +5904,11 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -5934,10 +5930,10 @@
         <v>101</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M37" t="s" s="2">
         <v>125</v>
@@ -5992,7 +5988,7 @@
         <v>46</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>44</v>
@@ -6030,7 +6026,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6053,13 +6049,13 @@
         <v>46</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="K38" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="K38" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -6110,7 +6106,7 @@
         <v>46</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>44</v>
@@ -6119,7 +6115,7 @@
         <v>56</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>68</v>
@@ -6134,10 +6130,10 @@
         <v>46</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>46</v>
@@ -6148,7 +6144,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6171,13 +6167,13 @@
         <v>46</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -6228,7 +6224,7 @@
         <v>46</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>44</v>
@@ -6237,7 +6233,7 @@
         <v>56</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>68</v>
@@ -6252,10 +6248,10 @@
         <v>46</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>46</v>
@@ -6266,7 +6262,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6292,16 +6288,16 @@
         <v>167</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>46</v>
@@ -6329,10 +6325,10 @@
         <v>80</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>46</v>
@@ -6350,7 +6346,7 @@
         <v>46</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>44</v>
@@ -6371,13 +6367,13 @@
         <v>46</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>46</v>
@@ -6388,7 +6384,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6414,16 +6410,16 @@
         <v>167</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="M41" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>46</v>
@@ -6448,13 +6444,13 @@
         <v>46</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>46</v>
@@ -6472,7 +6468,7 @@
         <v>46</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>44</v>
@@ -6493,13 +6489,13 @@
         <v>46</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>46</v>
@@ -6510,7 +6506,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6533,17 +6529,17 @@
         <v>46</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>46</v>
@@ -6592,7 +6588,7 @@
         <v>46</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>44</v>
@@ -6619,7 +6615,7 @@
         <v>46</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>46</v>
@@ -6630,7 +6626,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6656,10 +6652,10 @@
         <v>58</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6710,7 +6706,7 @@
         <v>46</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>44</v>
@@ -6734,10 +6730,10 @@
         <v>46</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>46</v>
@@ -6748,7 +6744,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6771,16 +6767,16 @@
         <v>57</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="K44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>384</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6830,7 +6826,7 @@
         <v>46</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>44</v>
@@ -6854,10 +6850,10 @@
         <v>46</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>46</v>
@@ -6868,7 +6864,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6891,16 +6887,16 @@
         <v>57</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="K45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6950,7 +6946,7 @@
         <v>46</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>44</v>
@@ -6974,10 +6970,10 @@
         <v>46</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>46</v>
@@ -6988,7 +6984,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7011,19 +7007,19 @@
         <v>57</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K46" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L46" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="N46" t="s" s="2">
         <v>394</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>396</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>46</v>
@@ -7072,7 +7068,7 @@
         <v>46</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>44</v>
@@ -7096,10 +7092,10 @@
         <v>46</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>46</v>
@@ -7110,7 +7106,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7136,10 +7132,10 @@
         <v>58</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -7190,7 +7186,7 @@
         <v>46</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>44</v>
@@ -7217,7 +7213,7 @@
         <v>46</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>46</v>
@@ -7228,7 +7224,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7254,10 +7250,10 @@
         <v>101</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>125</v>
@@ -7310,7 +7306,7 @@
         <v>46</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>44</v>
@@ -7337,7 +7333,7 @@
         <v>46</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>46</v>
@@ -7348,11 +7344,11 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7374,10 +7370,10 @@
         <v>101</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M49" t="s" s="2">
         <v>125</v>
@@ -7432,7 +7428,7 @@
         <v>46</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>44</v>
@@ -7470,7 +7466,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7496,16 +7492,16 @@
         <v>167</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L50" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="N50" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>46</v>
@@ -7530,13 +7526,13 @@
         <v>46</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>46</v>
@@ -7554,7 +7550,7 @@
         <v>46</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>56</v>
@@ -7575,16 +7571,16 @@
         <v>46</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AM50" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="AN50" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="AP50" t="s" s="2">
         <v>46</v>
@@ -7592,7 +7588,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7615,19 +7611,19 @@
         <v>57</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="L51" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>413</v>
-      </c>
       <c r="N51" t="s" s="2">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>46</v>
@@ -7676,7 +7672,7 @@
         <v>46</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>44</v>
@@ -7697,24 +7693,24 @@
         <v>46</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="AM51" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AO51" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AP51" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP51" t="s" s="2">
-        <v>260</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7740,16 +7736,16 @@
         <v>167</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="L52" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>418</v>
-      </c>
       <c r="N52" t="s" s="2">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>46</v>
@@ -7774,13 +7770,13 @@
         <v>46</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>46</v>
@@ -7798,7 +7794,7 @@
         <v>46</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>44</v>
@@ -7807,7 +7803,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>68</v>
@@ -7825,7 +7821,7 @@
         <v>99</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>46</v>
@@ -7836,11 +7832,11 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7862,16 +7858,16 @@
         <v>167</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="L53" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="N53" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>46</v>
@@ -7896,13 +7892,13 @@
         <v>46</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>46</v>
@@ -7920,7 +7916,7 @@
         <v>46</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>44</v>
@@ -7941,24 +7937,24 @@
         <v>46</v>
       </c>
       <c r="AL53" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AN53" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="AM53" t="s" s="2">
+      <c r="AO53" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="AP53" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="AN53" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AO53" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP53" t="s" s="2">
-        <v>278</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7984,16 +7980,16 @@
         <v>46</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>46</v>
@@ -8042,7 +8038,7 @@
         <v>46</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>44</v>
@@ -8066,10 +8062,10 @@
         <v>46</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>46</v>

</xml_diff>

<commit_message>
Fix QA errors and change for STU1
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="423">
   <si>
     <t>Path</t>
   </si>
@@ -607,7 +607,7 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>http://loinc.org</t>
+    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -782,7 +782,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">The person who performed the assessment. May also be used to provide the practitioner role and organization. </t>
+    <t>The person who performed the assessment. May also be used to provide the practitioner role and organization.</t>
   </si>
   <si>
     <t>Who was responsible for asserting the observed value as "true".</t>
@@ -1296,9 +1296,6 @@
   </si>
   <si>
     <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>&lt; 363787002 |Observable entity| OR @@ -1524,7 +1521,7 @@
     <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="104.1484375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="103.56640625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -7532,7 +7529,7 @@
         <v>404</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>405</v>
+        <v>186</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>46</v>
@@ -7571,7 +7568,7 @@
         <v>46</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>189</v>
@@ -7588,7 +7585,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7611,16 +7608,16 @@
         <v>57</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="L51" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>411</v>
       </c>
       <c r="N51" t="s" s="2">
         <v>252</v>
@@ -7672,7 +7669,7 @@
         <v>46</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>44</v>
@@ -7693,7 +7690,7 @@
         <v>46</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>256</v>
@@ -7710,7 +7707,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7736,13 +7733,13 @@
         <v>167</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>414</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>415</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>416</v>
       </c>
       <c r="N52" t="s" s="2">
         <v>262</v>
@@ -7773,7 +7770,7 @@
         <v>185</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Y52" t="s" s="2">
         <v>263</v>
@@ -7794,7 +7791,7 @@
         <v>46</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>44</v>
@@ -7803,7 +7800,7 @@
         <v>56</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>68</v>
@@ -7832,7 +7829,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7858,7 +7855,7 @@
         <v>167</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>268</v>
@@ -7916,7 +7913,7 @@
         <v>46</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>44</v>
@@ -7954,7 +7951,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7980,10 +7977,10 @@
         <v>46</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>322</v>
@@ -8038,7 +8035,7 @@
         <v>46</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>44</v>

</xml_diff>

<commit_message>
Add changes to resolve ballot comments
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="414">
   <si>
     <t>Path</t>
   </si>
@@ -775,6 +775,10 @@
   </si>
   <si>
     <t>Observation.value[x]</t>
+  </si>
+  <si>
+    <t>Quantity
+CodeableConcept</t>
   </si>
   <si>
     <t>Actual result</t>
@@ -4361,19 +4365,19 @@
         <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>166</v>
+        <v>242</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4431,7 +4435,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4440,24 +4444,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4486,13 +4490,13 @@
         <v>138</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4520,10 +4524,10 @@
         <v>171</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4541,7 +4545,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4550,7 +4554,7 @@
         <v>55</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>67</v>
@@ -4565,7 +4569,7 @@
         <v>98</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4576,11 +4580,11 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -4605,13 +4609,13 @@
         <v>138</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4639,10 +4643,10 @@
         <v>171</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4660,7 +4664,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4678,24 +4682,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4718,19 +4722,19 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4779,7 +4783,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4800,10 +4804,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4814,7 +4818,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4843,10 +4847,10 @@
         <v>138</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4872,13 +4876,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4896,7 +4900,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4914,24 +4918,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4960,13 +4964,13 @@
         <v>138</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -4991,13 +4995,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -5015,7 +5019,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5036,10 +5040,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5050,7 +5054,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5073,16 +5077,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K31" t="s" s="2">
         <v>138</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5132,7 +5136,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5150,24 +5154,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5190,16 +5194,16 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>138</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5249,7 +5253,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5267,24 +5271,24 @@
         <v>45</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5307,19 +5311,19 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="K33" t="s" s="2">
         <v>138</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5368,7 +5372,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5380,7 +5384,7 @@
         <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>45</v>
@@ -5389,10 +5393,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5403,7 +5407,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5429,10 +5433,10 @@
         <v>57</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5483,7 +5487,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5507,7 +5511,7 @@
         <v>45</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5518,7 +5522,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5544,10 +5548,10 @@
         <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M35" t="s" s="2">
         <v>123</v>
@@ -5600,7 +5604,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5624,7 +5628,7 @@
         <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5635,11 +5639,11 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -5661,10 +5665,10 @@
         <v>100</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="M36" t="s" s="2">
         <v>123</v>
@@ -5719,7 +5723,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5754,7 +5758,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5777,13 +5781,13 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5834,7 +5838,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5843,7 +5847,7 @@
         <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>67</v>
@@ -5855,10 +5859,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5869,7 +5873,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5892,13 +5896,13 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5949,7 +5953,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5958,7 +5962,7 @@
         <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>67</v>
@@ -5970,10 +5974,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5984,7 +5988,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6010,16 +6014,16 @@
         <v>166</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6047,10 +6051,10 @@
         <v>79</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6068,7 +6072,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6086,13 +6090,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6103,7 +6107,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6129,16 +6133,16 @@
         <v>166</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6163,13 +6167,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6187,7 +6191,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6205,13 +6209,13 @@
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6222,7 +6226,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6245,17 +6249,17 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6304,7 +6308,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6328,7 +6332,7 @@
         <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6339,7 +6343,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6365,10 +6369,10 @@
         <v>57</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6419,7 +6423,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6440,10 +6444,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6454,7 +6458,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6477,16 +6481,16 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6536,7 +6540,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6557,10 +6561,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6571,7 +6575,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6594,16 +6598,16 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6653,7 +6657,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6674,10 +6678,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6688,7 +6692,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6711,19 +6715,19 @@
         <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="K45" t="s" s="2">
         <v>138</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -6772,7 +6776,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6793,10 +6797,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6807,7 +6811,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6833,10 +6837,10 @@
         <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6887,7 +6891,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6911,7 +6915,7 @@
         <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6922,7 +6926,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6948,10 +6952,10 @@
         <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>123</v>
@@ -7004,7 +7008,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7028,7 +7032,7 @@
         <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7039,11 +7043,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7065,10 +7069,10 @@
         <v>100</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>123</v>
@@ -7123,7 +7127,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7158,7 +7162,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7184,13 +7188,13 @@
         <v>166</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="N49" t="s" s="2">
         <v>180</v>
@@ -7218,10 +7222,10 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="Y49" t="s" s="2">
         <v>181</v>
@@ -7242,7 +7246,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>55</v>
@@ -7260,7 +7264,7 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>184</v>
@@ -7277,7 +7281,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7300,19 +7304,19 @@
         <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7361,7 +7365,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7379,24 +7383,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7422,16 +7426,16 @@
         <v>166</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7459,10 +7463,10 @@
         <v>171</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7480,7 +7484,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7489,7 +7493,7 @@
         <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>67</v>
@@ -7504,7 +7508,7 @@
         <v>98</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7515,11 +7519,11 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7541,16 +7545,16 @@
         <v>166</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7578,10 +7582,10 @@
         <v>171</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7599,7 +7603,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7617,24 +7621,24 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7660,16 +7664,16 @@
         <v>45</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7718,7 +7722,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7739,10 +7743,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Update for addressing ballot issues
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-bcs.xlsx
+++ b/build/output/StructureDefinition-pacio-bcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="413">
   <si>
     <t>Path</t>
   </si>
@@ -778,7 +778,7 @@
   </si>
   <si>
     <t>Quantity
-CodeableConcept</t>
+CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual result</t>
@@ -1277,10 +1277,6 @@
   </si>
   <si>
     <t>Observation.component.value[x]</t>
-  </si>
-  <si>
-    <t>Quantity
-CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual component result</t>
@@ -7304,16 +7300,16 @@
         <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K50" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="L50" t="s" s="2">
         <v>244</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N50" t="s" s="2">
         <v>246</v>
@@ -7383,7 +7379,7 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>249</v>
@@ -7400,7 +7396,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7426,13 +7422,13 @@
         <v>166</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>406</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>407</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>408</v>
       </c>
       <c r="N51" t="s" s="2">
         <v>255</v>
@@ -7484,7 +7480,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7519,7 +7515,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7545,7 +7541,7 @@
         <v>166</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L52" t="s" s="2">
         <v>262</v>
@@ -7603,7 +7599,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7638,7 +7634,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7664,10 +7660,10 @@
         <v>45</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="M53" t="s" s="2">
         <v>316</v>
@@ -7722,7 +7718,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>

</xml_diff>